<commit_message>
edit dashboard & data
</commit_message>
<xml_diff>
--- a/public/Data/data_import.xlsx
+++ b/public/Data/data_import.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinkakharismaadzania/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EFC930F-B557-D644-B776-B063882C5EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18DF2F73-B1EB-0B43-A7A9-6E93C933E17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1780" windowWidth="28800" windowHeight="10620" xr2:uid="{695C5FAD-43E1-A347-81F7-32E96ECB116C}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="16300" windowHeight="16480" xr2:uid="{695C5FAD-43E1-A347-81F7-32E96ECB116C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$2128</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -396,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0D483BF-D772-884D-81DB-C57F3E8C3895}">
-  <dimension ref="A1:I2190"/>
+  <dimension ref="A1:I2128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2121" workbookViewId="0">
-      <selection activeCell="K2130" sqref="K2130"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -62116,193 +62119,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2129" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2129" s="1"/>
-    </row>
-    <row r="2130" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2130" s="1"/>
-    </row>
-    <row r="2131" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2131" s="1"/>
-    </row>
-    <row r="2132" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2132" s="1"/>
-    </row>
-    <row r="2133" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2133" s="1"/>
-    </row>
-    <row r="2134" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2134" s="1"/>
-    </row>
-    <row r="2135" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2135" s="1"/>
-    </row>
-    <row r="2136" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2136" s="1"/>
-    </row>
-    <row r="2137" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2137" s="1"/>
-    </row>
-    <row r="2138" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2138" s="1"/>
-    </row>
-    <row r="2139" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2139" s="1"/>
-    </row>
-    <row r="2140" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2140" s="1"/>
-    </row>
-    <row r="2141" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2141" s="1"/>
-    </row>
-    <row r="2142" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2142" s="1"/>
-    </row>
-    <row r="2143" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2143" s="1"/>
-    </row>
-    <row r="2144" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2144" s="1"/>
-    </row>
-    <row r="2145" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2145" s="1"/>
-    </row>
-    <row r="2146" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2146" s="1"/>
-    </row>
-    <row r="2147" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2147" s="1"/>
-    </row>
-    <row r="2148" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2148" s="1"/>
-    </row>
-    <row r="2149" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2149" s="1"/>
-    </row>
-    <row r="2150" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2150" s="1"/>
-    </row>
-    <row r="2151" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2151" s="1"/>
-    </row>
-    <row r="2152" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2152" s="1"/>
-    </row>
-    <row r="2153" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2153" s="1"/>
-    </row>
-    <row r="2154" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2154" s="1"/>
-    </row>
-    <row r="2155" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2155" s="1"/>
-    </row>
-    <row r="2156" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2156" s="1"/>
-    </row>
-    <row r="2157" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2157" s="1"/>
-    </row>
-    <row r="2158" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2158" s="1"/>
-    </row>
-    <row r="2159" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2159" s="1"/>
-    </row>
-    <row r="2160" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2160" s="1"/>
-    </row>
-    <row r="2161" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2161" s="1"/>
-    </row>
-    <row r="2162" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2162" s="1"/>
-    </row>
-    <row r="2163" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2163" s="1"/>
-    </row>
-    <row r="2164" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2164" s="1"/>
-    </row>
-    <row r="2165" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2165" s="1"/>
-    </row>
-    <row r="2166" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2166" s="1"/>
-    </row>
-    <row r="2167" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2167" s="1"/>
-    </row>
-    <row r="2168" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2168" s="1"/>
-    </row>
-    <row r="2169" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2169" s="1"/>
-    </row>
-    <row r="2170" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2170" s="1"/>
-    </row>
-    <row r="2171" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2171" s="1"/>
-    </row>
-    <row r="2172" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2172" s="1"/>
-    </row>
-    <row r="2173" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2173" s="1"/>
-    </row>
-    <row r="2174" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2174" s="1"/>
-    </row>
-    <row r="2175" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2175" s="1"/>
-    </row>
-    <row r="2176" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2176" s="1"/>
-    </row>
-    <row r="2177" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2177" s="1"/>
-    </row>
-    <row r="2178" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2178" s="1"/>
-    </row>
-    <row r="2179" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2179" s="1"/>
-    </row>
-    <row r="2180" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2180" s="1"/>
-    </row>
-    <row r="2181" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2181" s="1"/>
-    </row>
-    <row r="2182" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2182" s="1"/>
-    </row>
-    <row r="2183" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2183" s="1"/>
-    </row>
-    <row r="2184" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2184" s="1"/>
-    </row>
-    <row r="2185" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2185" s="1"/>
-    </row>
-    <row r="2186" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2186" s="1"/>
-    </row>
-    <row r="2187" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2187" s="1"/>
-    </row>
-    <row r="2188" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2188" s="1"/>
-    </row>
-    <row r="2189" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2189" s="1"/>
-    </row>
-    <row r="2190" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B2190" s="1"/>
-    </row>
   </sheetData>
+  <autoFilter ref="C1:C2128" xr:uid="{A0D483BF-D772-884D-81DB-C57F3E8C3895}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>